<commit_message>
[FINISH] Homework Wk11 - Latihan 1 - Toko Barang - Latihan 2 - Toko Bunga
</commit_message>
<xml_diff>
--- a/homework/bab_08/Modul8-10116122.xlsx
+++ b/homework/bab_08/Modul8-10116122.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13620" windowHeight="15280" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="15280" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabel - Latihan 1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabel - Latihan 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="MochamadIqbalDwiCahyo">'Tabel - Latihan 2'!$B$2:$D$6</definedName>
-    <definedName name="N10116122">'Tabel - Latihan 2'!$F$2:$H$4</definedName>
-    <definedName name="NIM10116122">'Tabel - Latihan 1'!$C$3:$G$4</definedName>
+    <definedName name="Lat1_10116122">'Tabel - Latihan 1'!$C$3:$G$4</definedName>
+    <definedName name="Lat1_MochamadIqbalDwiCahyo">'Tabel - Latihan 1'!$C$7:$E$11</definedName>
+    <definedName name="Lat2_10116122">'Tabel - Latihan 2'!$B$2:$D$6</definedName>
+    <definedName name="Lat2_MochamadIqbalDwiCahyo">'Tabel - Latihan 2'!$F$2:$H$4</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -409,13 +410,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency [0]" xfId="1" builtinId="7"/>
@@ -697,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I27"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -812,22 +813,22 @@
       <c r="I11" s="4"/>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="12"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="12"/>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="12"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
@@ -865,23 +866,23 @@
       <c r="D18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="1" t="e">
-        <f t="shared" ref="E18:E27" si="0">VLOOKUP($D18,MochamadIqbalDwiCahyo,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F18" s="5" t="e">
-        <f t="shared" ref="F18:F27" si="1">VLOOKUP($D18,MochamadIqbalDwiCahyo,3,0)</f>
-        <v>#N/A</v>
+      <c r="E18" s="1" t="str">
+        <f>VLOOKUP($D18,Lat1_MochamadIqbalDwiCahyo,2,0)</f>
+        <v>1 Set Alat Kantor</v>
+      </c>
+      <c r="F18" s="5">
+        <f>VLOOKUP($D18,Lat1_MochamadIqbalDwiCahyo,3,0)</f>
+        <v>5000000</v>
       </c>
       <c r="G18" s="1">
         <v>5</v>
       </c>
-      <c r="H18" s="5" t="e">
+      <c r="H18" s="5">
         <f>$F18*$G18</f>
-        <v>#N/A</v>
+        <v>25000000</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f t="shared" ref="I18:I27" si="2">HLOOKUP($D18,NIM10116122,2,0)</f>
+        <f>HLOOKUP($D18,Lat1_10116122,2,0)</f>
         <v>Kertas 4 Rim</v>
       </c>
     </row>
@@ -895,23 +896,23 @@
       <c r="D19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F19" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
+      <c r="E19" s="1" t="str">
+        <f>VLOOKUP($D19,Lat1_MochamadIqbalDwiCahyo,2,0)</f>
+        <v>Printer Canon BJ 100 SP</v>
+      </c>
+      <c r="F19" s="5">
+        <f>VLOOKUP($D19,Lat1_MochamadIqbalDwiCahyo,3,0)</f>
+        <v>7500000</v>
       </c>
       <c r="G19" s="1">
         <v>7</v>
       </c>
-      <c r="H19" s="5" t="e">
-        <f t="shared" ref="H19:H27" si="3">$F19*$G19</f>
-        <v>#N/A</v>
+      <c r="H19" s="5">
+        <f t="shared" ref="H19:H27" si="0">$F19*$G19</f>
+        <v>52500000</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>HLOOKUP($D19,Lat1_10116122,2,0)</f>
         <v>Tinta Refill Inkjet</v>
       </c>
     </row>
@@ -925,23 +926,23 @@
       <c r="D20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F20" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
+      <c r="E20" s="1" t="str">
+        <f>VLOOKUP($D20,Lat1_MochamadIqbalDwiCahyo,2,0)</f>
+        <v>Buku Tulis Kantor</v>
+      </c>
+      <c r="F20" s="5">
+        <f>VLOOKUP($D20,Lat1_MochamadIqbalDwiCahyo,3,0)</f>
+        <v>2500000</v>
       </c>
       <c r="G20" s="1">
         <v>3</v>
       </c>
-      <c r="H20" s="5" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
+      <c r="H20" s="5">
+        <f t="shared" si="0"/>
+        <v>7500000</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>HLOOKUP($D20,Lat1_10116122,2,0)</f>
         <v>Sampel Buku</v>
       </c>
     </row>
@@ -955,23 +956,23 @@
       <c r="D21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F21" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
+      <c r="E21" s="1" t="str">
+        <f>VLOOKUP($D21,Lat1_MochamadIqbalDwiCahyo,2,0)</f>
+        <v>Kertas Bola Dunia</v>
+      </c>
+      <c r="F21" s="5">
+        <f>VLOOKUP($D21,Lat1_MochamadIqbalDwiCahyo,3,0)</f>
+        <v>3450000</v>
       </c>
       <c r="G21" s="1">
         <v>4</v>
       </c>
-      <c r="H21" s="5" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
+      <c r="H21" s="5">
+        <f t="shared" si="0"/>
+        <v>13800000</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>HLOOKUP($D21,Lat1_10116122,2,0)</f>
         <v>Gunting</v>
       </c>
     </row>
@@ -985,23 +986,23 @@
       <c r="D22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F22" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
+      <c r="E22" s="1" t="str">
+        <f>VLOOKUP($D22,Lat1_MochamadIqbalDwiCahyo,2,0)</f>
+        <v>1 Set Alat Kantor</v>
+      </c>
+      <c r="F22" s="5">
+        <f>VLOOKUP($D22,Lat1_MochamadIqbalDwiCahyo,3,0)</f>
+        <v>5000000</v>
       </c>
       <c r="G22" s="1">
         <v>9</v>
       </c>
-      <c r="H22" s="5" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
+      <c r="H22" s="5">
+        <f t="shared" si="0"/>
+        <v>45000000</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>HLOOKUP($D22,Lat1_10116122,2,0)</f>
         <v>Kertas 4 Rim</v>
       </c>
     </row>
@@ -1015,23 +1016,23 @@
       <c r="D23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F23" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
+      <c r="E23" s="1" t="str">
+        <f>VLOOKUP($D23,Lat1_MochamadIqbalDwiCahyo,2,0)</f>
+        <v>Printer Canon BJ 100 SP</v>
+      </c>
+      <c r="F23" s="5">
+        <f>VLOOKUP($D23,Lat1_MochamadIqbalDwiCahyo,3,0)</f>
+        <v>7500000</v>
       </c>
       <c r="G23" s="1">
         <v>10</v>
       </c>
-      <c r="H23" s="5" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
+      <c r="H23" s="5">
+        <f t="shared" si="0"/>
+        <v>75000000</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>HLOOKUP($D23,Lat1_10116122,2,0)</f>
         <v>Tinta Refill Inkjet</v>
       </c>
     </row>
@@ -1045,23 +1046,23 @@
       <c r="D24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F24" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
+      <c r="E24" s="1" t="str">
+        <f>VLOOKUP($D24,Lat1_MochamadIqbalDwiCahyo,2,0)</f>
+        <v>Buku Tulis Kantor</v>
+      </c>
+      <c r="F24" s="5">
+        <f>VLOOKUP($D24,Lat1_MochamadIqbalDwiCahyo,3,0)</f>
+        <v>2500000</v>
       </c>
       <c r="G24" s="1">
         <v>6</v>
       </c>
-      <c r="H24" s="5" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
+      <c r="H24" s="5">
+        <f t="shared" si="0"/>
+        <v>15000000</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>HLOOKUP($D24,Lat1_10116122,2,0)</f>
         <v>Sampel Buku</v>
       </c>
     </row>
@@ -1075,23 +1076,23 @@
       <c r="D25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F25" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
+      <c r="E25" s="1" t="str">
+        <f>VLOOKUP($D25,Lat1_MochamadIqbalDwiCahyo,2,0)</f>
+        <v>Kertas Bola Dunia</v>
+      </c>
+      <c r="F25" s="5">
+        <f>VLOOKUP($D25,Lat1_MochamadIqbalDwiCahyo,3,0)</f>
+        <v>3450000</v>
       </c>
       <c r="G25" s="1">
         <v>5</v>
       </c>
-      <c r="H25" s="5" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
+      <c r="H25" s="5">
+        <f t="shared" si="0"/>
+        <v>17250000</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>HLOOKUP($D25,Lat1_10116122,2,0)</f>
         <v>Gunting</v>
       </c>
     </row>
@@ -1105,23 +1106,23 @@
       <c r="D26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F26" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
+      <c r="E26" s="1" t="str">
+        <f>VLOOKUP($D26,Lat1_MochamadIqbalDwiCahyo,2,0)</f>
+        <v>Kertas Bola Dunia</v>
+      </c>
+      <c r="F26" s="5">
+        <f>VLOOKUP($D26,Lat1_MochamadIqbalDwiCahyo,3,0)</f>
+        <v>3450000</v>
       </c>
       <c r="G26" s="1">
         <v>3</v>
       </c>
-      <c r="H26" s="5" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
+      <c r="H26" s="5">
+        <f t="shared" si="0"/>
+        <v>10350000</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>HLOOKUP($D26,Lat1_10116122,2,0)</f>
         <v>Gunting</v>
       </c>
     </row>
@@ -1135,23 +1136,23 @@
       <c r="D27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F27" s="5" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
+      <c r="E27" s="1" t="str">
+        <f>VLOOKUP($D27,Lat1_MochamadIqbalDwiCahyo,2,0)</f>
+        <v>1 Set Alat Kantor</v>
+      </c>
+      <c r="F27" s="5">
+        <f>VLOOKUP($D27,Lat1_MochamadIqbalDwiCahyo,3,0)</f>
+        <v>5000000</v>
       </c>
       <c r="G27" s="1">
         <v>4</v>
       </c>
-      <c r="H27" s="5" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
+      <c r="H27" s="5">
+        <f t="shared" si="0"/>
+        <v>20000000</v>
       </c>
       <c r="I27" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>HLOOKUP($D27,Lat1_10116122,2,0)</f>
         <v>Kertas 4 Rim</v>
       </c>
     </row>
@@ -1175,7 +1176,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12:J21"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1219,8 +1220,8 @@
       <c r="H2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
@@ -1238,12 +1239,12 @@
       <c r="G3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="10">
         <f>15/100</f>
         <v>0.15</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
@@ -1261,7 +1262,7 @@
       <c r="G4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <f>2/100</f>
         <v>0.02</v>
       </c>
@@ -1289,12 +1290,12 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1353,11 +1354,11 @@
         <v>82</v>
       </c>
       <c r="F12" s="1" t="str">
-        <f>VLOOKUP(MID($D12,4,2),MochamadIqbalDwiCahyo,2,0)</f>
+        <f>VLOOKUP(MID($D12,4,2),Lat2_10116122,2,0)</f>
         <v>Lokal</v>
       </c>
       <c r="G12" s="5">
-        <f>VLOOKUP(MID($D12,4,2),MochamadIqbalDwiCahyo,3,0)</f>
+        <f>VLOOKUP(MID($D12,4,2),Lat2_10116122,3,0)</f>
         <v>40000</v>
       </c>
       <c r="H12" s="1">
@@ -1368,10 +1369,10 @@
         <v>560000</v>
       </c>
       <c r="J12" s="5">
-        <f>(VLOOKUP(LEFT($B12,3),N10116122,3,0)*$I12)</f>
+        <f>(VLOOKUP(LEFT($B12,3),Lat2_MochamadIqbalDwiCahyo,3,0)*$I12)</f>
         <v>84000</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="11">
         <f>$I12-$J12</f>
         <v>476000</v>
       </c>
@@ -1393,11 +1394,11 @@
         <v>83</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f>VLOOKUP(MID($D13,4,2),MochamadIqbalDwiCahyo,2,0)</f>
+        <f>VLOOKUP(MID($D13,4,2),Lat2_10116122,2,0)</f>
         <v>Import</v>
       </c>
       <c r="G13" s="5">
-        <f>VLOOKUP(MID($D13,4,2),MochamadIqbalDwiCahyo,3,0)</f>
+        <f>VLOOKUP(MID($D13,4,2),Lat2_10116122,3,0)</f>
         <v>89000</v>
       </c>
       <c r="H13" s="1">
@@ -1408,10 +1409,10 @@
         <v>1780000</v>
       </c>
       <c r="J13" s="5">
-        <f>(VLOOKUP(LEFT($B13,3),N10116122,3,0)*$I13)</f>
+        <f>(VLOOKUP(LEFT($B13,3),Lat2_MochamadIqbalDwiCahyo,3,0)*$I13)</f>
         <v>35600</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="11">
         <f t="shared" ref="K13:K21" si="1">$I13-$J13</f>
         <v>1744400</v>
       </c>
@@ -1433,11 +1434,11 @@
         <v>84</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f>VLOOKUP(MID($D14,4,2),MochamadIqbalDwiCahyo,2,0)</f>
+        <f>VLOOKUP(MID($D14,4,2),Lat2_10116122,2,0)</f>
         <v>Kawinan</v>
       </c>
       <c r="G14" s="5">
-        <f>VLOOKUP(MID($D14,4,2),MochamadIqbalDwiCahyo,3,0)</f>
+        <f>VLOOKUP(MID($D14,4,2),Lat2_10116122,3,0)</f>
         <v>78000</v>
       </c>
       <c r="H14" s="1">
@@ -1448,10 +1449,10 @@
         <v>702000</v>
       </c>
       <c r="J14" s="5">
-        <f>(VLOOKUP(LEFT($B14,3),N10116122,3,0)*$I14)</f>
+        <f>(VLOOKUP(LEFT($B14,3),Lat2_MochamadIqbalDwiCahyo,3,0)*$I14)</f>
         <v>105300</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="11">
         <f t="shared" si="1"/>
         <v>596700</v>
       </c>
@@ -1473,11 +1474,11 @@
         <v>85</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f>VLOOKUP(MID($D15,4,2),MochamadIqbalDwiCahyo,2,0)</f>
+        <f>VLOOKUP(MID($D15,4,2),Lat2_10116122,2,0)</f>
         <v>Campuran</v>
       </c>
       <c r="G15" s="5">
-        <f>VLOOKUP(MID($D15,4,2),MochamadIqbalDwiCahyo,3,0)</f>
+        <f>VLOOKUP(MID($D15,4,2),Lat2_10116122,3,0)</f>
         <v>120000</v>
       </c>
       <c r="H15" s="1">
@@ -1488,10 +1489,10 @@
         <v>2760000</v>
       </c>
       <c r="J15" s="5">
-        <f>(VLOOKUP(LEFT($B15,3),N10116122,3,0)*$I15)</f>
+        <f>(VLOOKUP(LEFT($B15,3),Lat2_MochamadIqbalDwiCahyo,3,0)*$I15)</f>
         <v>55200</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K15" s="11">
         <f t="shared" si="1"/>
         <v>2704800</v>
       </c>
@@ -1513,11 +1514,11 @@
         <v>86</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>VLOOKUP(MID($D16,4,2),MochamadIqbalDwiCahyo,2,0)</f>
+        <f>VLOOKUP(MID($D16,4,2),Lat2_10116122,2,0)</f>
         <v>Lokal</v>
       </c>
       <c r="G16" s="5">
-        <f>VLOOKUP(MID($D16,4,2),MochamadIqbalDwiCahyo,3,0)</f>
+        <f>VLOOKUP(MID($D16,4,2),Lat2_10116122,3,0)</f>
         <v>40000</v>
       </c>
       <c r="H16" s="1">
@@ -1528,10 +1529,10 @@
         <v>400000</v>
       </c>
       <c r="J16" s="5">
-        <f>(VLOOKUP(LEFT($B16,3),N10116122,3,0)*$I16)</f>
+        <f>(VLOOKUP(LEFT($B16,3),Lat2_MochamadIqbalDwiCahyo,3,0)*$I16)</f>
         <v>60000</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="11">
         <f t="shared" si="1"/>
         <v>340000</v>
       </c>
@@ -1553,11 +1554,11 @@
         <v>87</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f>VLOOKUP(MID($D17,4,2),MochamadIqbalDwiCahyo,2,0)</f>
+        <f>VLOOKUP(MID($D17,4,2),Lat2_10116122,2,0)</f>
         <v>Import</v>
       </c>
       <c r="G17" s="5">
-        <f>VLOOKUP(MID($D17,4,2),MochamadIqbalDwiCahyo,3,0)</f>
+        <f>VLOOKUP(MID($D17,4,2),Lat2_10116122,3,0)</f>
         <v>89000</v>
       </c>
       <c r="H17" s="1">
@@ -1568,10 +1569,10 @@
         <v>1068000</v>
       </c>
       <c r="J17" s="5">
-        <f>(VLOOKUP(LEFT($B17,3),N10116122,3,0)*$I17)</f>
+        <f>(VLOOKUP(LEFT($B17,3),Lat2_MochamadIqbalDwiCahyo,3,0)*$I17)</f>
         <v>21360</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="11">
         <f t="shared" si="1"/>
         <v>1046640</v>
       </c>
@@ -1593,11 +1594,11 @@
         <v>88</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f>VLOOKUP(MID($D18,4,2),MochamadIqbalDwiCahyo,2,0)</f>
+        <f>VLOOKUP(MID($D18,4,2),Lat2_10116122,2,0)</f>
         <v>Kawinan</v>
       </c>
       <c r="G18" s="5">
-        <f>VLOOKUP(MID($D18,4,2),MochamadIqbalDwiCahyo,3,0)</f>
+        <f>VLOOKUP(MID($D18,4,2),Lat2_10116122,3,0)</f>
         <v>78000</v>
       </c>
       <c r="H18" s="1">
@@ -1608,10 +1609,10 @@
         <v>858000</v>
       </c>
       <c r="J18" s="5">
-        <f>(VLOOKUP(LEFT($B18,3),N10116122,3,0)*$I18)</f>
+        <f>(VLOOKUP(LEFT($B18,3),Lat2_MochamadIqbalDwiCahyo,3,0)*$I18)</f>
         <v>128700</v>
       </c>
-      <c r="K18" s="12">
+      <c r="K18" s="11">
         <f t="shared" si="1"/>
         <v>729300</v>
       </c>
@@ -1633,11 +1634,11 @@
         <v>89</v>
       </c>
       <c r="F19" s="1" t="str">
-        <f>VLOOKUP(MID($D19,4,2),MochamadIqbalDwiCahyo,2,0)</f>
+        <f>VLOOKUP(MID($D19,4,2),Lat2_10116122,2,0)</f>
         <v>Campuran</v>
       </c>
       <c r="G19" s="5">
-        <f>VLOOKUP(MID($D19,4,2),MochamadIqbalDwiCahyo,3,0)</f>
+        <f>VLOOKUP(MID($D19,4,2),Lat2_10116122,3,0)</f>
         <v>120000</v>
       </c>
       <c r="H19" s="1">
@@ -1648,10 +1649,10 @@
         <v>840000</v>
       </c>
       <c r="J19" s="5">
-        <f>(VLOOKUP(LEFT($B19,3),N10116122,3,0)*$I19)</f>
+        <f>(VLOOKUP(LEFT($B19,3),Lat2_MochamadIqbalDwiCahyo,3,0)*$I19)</f>
         <v>16800</v>
       </c>
-      <c r="K19" s="12">
+      <c r="K19" s="11">
         <f t="shared" si="1"/>
         <v>823200</v>
       </c>
@@ -1673,11 +1674,11 @@
         <v>90</v>
       </c>
       <c r="F20" s="1" t="str">
-        <f>VLOOKUP(MID($D20,4,2),MochamadIqbalDwiCahyo,2,0)</f>
+        <f>VLOOKUP(MID($D20,4,2),Lat2_10116122,2,0)</f>
         <v>Lokal</v>
       </c>
       <c r="G20" s="5">
-        <f>VLOOKUP(MID($D20,4,2),MochamadIqbalDwiCahyo,3,0)</f>
+        <f>VLOOKUP(MID($D20,4,2),Lat2_10116122,3,0)</f>
         <v>40000</v>
       </c>
       <c r="H20" s="1">
@@ -1688,10 +1689,10 @@
         <v>240000</v>
       </c>
       <c r="J20" s="5">
-        <f>(VLOOKUP(LEFT($B20,3),N10116122,3,0)*$I20)</f>
+        <f>(VLOOKUP(LEFT($B20,3),Lat2_MochamadIqbalDwiCahyo,3,0)*$I20)</f>
         <v>36000</v>
       </c>
-      <c r="K20" s="12">
+      <c r="K20" s="11">
         <f t="shared" si="1"/>
         <v>204000</v>
       </c>
@@ -1713,11 +1714,11 @@
         <v>82</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f>VLOOKUP(MID($D21,4,2),MochamadIqbalDwiCahyo,2,0)</f>
+        <f>VLOOKUP(MID($D21,4,2),Lat2_10116122,2,0)</f>
         <v>Lokal</v>
       </c>
       <c r="G21" s="5">
-        <f>VLOOKUP(MID($D21,4,2),MochamadIqbalDwiCahyo,3,0)</f>
+        <f>VLOOKUP(MID($D21,4,2),Lat2_10116122,3,0)</f>
         <v>40000</v>
       </c>
       <c r="H21" s="1">
@@ -1728,10 +1729,10 @@
         <v>240000</v>
       </c>
       <c r="J21" s="5">
-        <f>(VLOOKUP(LEFT($B21,3),N10116122,3,0)*$I21)</f>
+        <f>(VLOOKUP(LEFT($B21,3),Lat2_MochamadIqbalDwiCahyo,3,0)*$I21)</f>
         <v>36000</v>
       </c>
-      <c r="K21" s="12">
+      <c r="K21" s="11">
         <f t="shared" si="1"/>
         <v>204000</v>
       </c>

</xml_diff>